<commit_message>
feat(Excel): Generate cell ranges
</commit_message>
<xml_diff>
--- a/Excel/out/test.xlsx
+++ b/Excel/out/test.xlsx
@@ -6,15 +6,40 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" sheetId="1" r:id="rId3"/>
+    <sheet name="Main" sheetId="1" r:id="rId3"/>
+    <sheet name="Investments" sheetId="2" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">Hello World</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment 100L cost per unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment 100L units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
   </si>
 </sst>
 </file>
@@ -64,12 +89,124 @@
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>$A$1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>INDIRECT(ADDRESS(5, 2))</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>$A$1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>INDIRECT(ADDRESS(5, 2))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>